<commit_message>
wedge tests continued A, B, C
</commit_message>
<xml_diff>
--- a/Jupyter/Wedge/prism_data_openmc.xlsx
+++ b/Jupyter/Wedge/prism_data_openmc.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MCNP\emma-openmc\Jupyter\Wedge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C7B4CC-608C-4954-BD0E-4BE3276E22A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A2FE34-9589-4D78-B56C-1ED4E59D4D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Figures" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,21 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Fertile kg/m3</t>
   </si>
   <si>
     <t>BISO/cm3</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>RESULTS</t>
@@ -96,6 +88,24 @@
   </si>
   <si>
     <t>factor</t>
+  </si>
+  <si>
+    <t>A-OpenMC</t>
+  </si>
+  <si>
+    <t>A-MCNP</t>
+  </si>
+  <si>
+    <t>B-OpenMC</t>
+  </si>
+  <si>
+    <t>B-MCNP</t>
+  </si>
+  <si>
+    <t>C-OpenMC</t>
+  </si>
+  <si>
+    <t>C-MCNP</t>
   </si>
 </sst>
 </file>
@@ -168,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -184,7 +194,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -201,6 +210,1734 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>D-shape</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$H$4:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.52725672373683E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.76088265923015E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2684723504348998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.02535867346246E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.6096776712520909E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7956202904139199E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.54716677488637E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2417642839879697E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9055212834252402E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.8983323870902299E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.103595084893309</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14519436153500101</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.185920101577397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000015-4742-4BCE-9B80-3DBD1BDD66B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>A-OpenMC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$I$4:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>3.5162900000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7669699999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.2894699999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0301599999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.5466400000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.7839399999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5426299999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.2291500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.9017400000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.9058800000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.104042</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14546899999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.186667</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000016-4742-4BCE-9B80-3DBD1BDD66B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>A-MCNP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$J$4:$J$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000017-4742-4BCE-9B80-3DBD1BDD66B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>B-OpenMC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$4:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.2188300000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4790399999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.07774E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.837540000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9574700000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.77656E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.35463E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2558700000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6777399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3802999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7241999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7511500000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000018-4742-4BCE-9B80-3DBD1BDD66B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>B-MCNP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$L$4:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>7.2283589800322982E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5506773449112674E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0564601677004478E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0548236927556496E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0948517588691182E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.108953764066098E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0812610365238457E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.017270967046913E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8697824484955642E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5481580872935446E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.136209612868915E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1478387405910621E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0537614166508758E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000019-4742-4BCE-9B80-3DBD1BDD66B3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1694165648"/>
+        <c:axId val="1694171408"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1694165648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694171408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1694171408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694165648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.84522394280705315"/>
+          <c:y val="0.35512939678475508"/>
+          <c:w val="0.10580624061480107"/>
+          <c:h val="0.24708902486800682"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>B-OpenMC</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$K$4:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>6.2188300000000001E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4790399999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.07774E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.837540000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9574700000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.77656E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.35463E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.2558700000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.6777399999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3802999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.7241999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.7511500000000003E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-28AC-48C1-9970-46F3FE5F96AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>B-MCNP</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet2!$A$4:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet2!$L$4:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>7.2283589800322982E-6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.5506773449112674E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0564601677004478E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.0548236927556496E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.0948517588691182E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.108953764066098E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.0812610365238457E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.017270967046913E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.8697824484955642E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5481580872935446E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.136209612868915E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.1478387405910621E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0537614166508758E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000E-28AC-48C1-9970-46F3FE5F96AC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1694165648"/>
+        <c:axId val="1694171408"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="5"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>D-shape</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="19050">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$4:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>750</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$H$4:$H$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>3.52725672373683E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.76088265923015E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.2684723504348998E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.02535867346246E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>9.6096776712520909E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.7956202904139199E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.54716677488637E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.2417642839879697E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.9055212834252402E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>5.8983323870902299E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.103595084893309</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.14519436153500101</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.185920101577397</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000000-28AC-48C1-9970-46F3FE5F96AC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>A-OpenMC</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400">
+                    <a:noFill/>
+                  </a:ln>
+                </c:spPr>
+                <c:trendline>
+                  <c:spPr>
+                    <a:ln w="19050" cap="rnd">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:prstDash val="sysDot"/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:trendlineType val="poly"/>
+                  <c:order val="4"/>
+                  <c:dispRSqr val="0"/>
+                  <c:dispEq val="0"/>
+                </c:trendline>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$4:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>750</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$I$4:$I$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>3.5162900000000002E-5</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1.7669699999999999E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>5.2894699999999999E-4</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>5.0301599999999997E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>9.5466400000000003E-3</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1.7839399999999998E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2.5426299999999999E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>3.2291500000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>3.9017400000000001E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>5.9058800000000002E-2</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>0.104042</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>0.14546899999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>0.186667</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000007-28AC-48C1-9970-46F3FE5F96AC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+            <c15:filteredScatterSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:v>A-MCNP</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="25400" cap="rnd">
+                    <a:noFill/>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:xVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$A$4:$A$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="13"/>
+                      <c:pt idx="0">
+                        <c:v>0.1</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>0.5</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1.5</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>30</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>60</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>90</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>120</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>150</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>250</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>500</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>750</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:xVal>
+                <c:yVal>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet2!$J$4:$J$16</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="13"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:yVal>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000008-28AC-48C1-9970-46F3FE5F96AC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredScatterSeries>
+          </c:ext>
+        </c:extLst>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1694165648"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0"/>
+                  <a:t>Fertile kg/m</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" baseline="30000"/>
+                  <a:t>3</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694171408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1694171408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" b="0"/>
+                  <a:t>U-238</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="0" baseline="0"/>
+                  <a:t> (n,gamma) reaction rate [rxns/src-n]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1694165648"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82640789834721173"/>
+          <c:y val="0.32271508700839524"/>
+          <c:w val="0.10580624061480107"/>
+          <c:h val="0.14395238402399732"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln w="6350">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>81474</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>139501</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>66236</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>87158</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C5A0AA4-A231-39CB-978B-A8D6B953BDB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114302</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>176257</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B723F39-E913-4D80-9A04-2B4CC4722B7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -466,10 +2203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A58FC2A7-2007-48F8-8A3D-08B47124466B}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N22" sqref="N22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U51" sqref="U51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -480,34 +2217,37 @@
     <col min="5" max="6" width="8" customWidth="1"/>
     <col min="7" max="7" width="2.109375" customWidth="1"/>
     <col min="8" max="8" width="10.88671875" customWidth="1"/>
-    <col min="9" max="11" width="10.44140625" customWidth="1"/>
-    <col min="12" max="12" width="1.77734375" customWidth="1"/>
-    <col min="13" max="13" width="8.6640625" customWidth="1"/>
-    <col min="14" max="14" width="9.44140625" customWidth="1"/>
-    <col min="15" max="15" width="8.33203125" customWidth="1"/>
-    <col min="16" max="16" width="2.77734375" customWidth="1"/>
+    <col min="9" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="14" width="10.44140625" customWidth="1"/>
+    <col min="15" max="15" width="1.77734375" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" customWidth="1"/>
+    <col min="17" max="17" width="9.44140625" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="H2" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="P2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
     </row>
-    <row r="3" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -515,42 +2255,51 @@
         <v>1</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P3" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="R3" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M3" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="N3" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="16" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>0.1</v>
       </c>
       <c r="B4" s="10">
-        <f>A4*$I$27</f>
+        <f>A4*$B$21</f>
         <v>4.0296735505064935E-2</v>
       </c>
       <c r="C4" s="10">
@@ -569,30 +2318,35 @@
       <c r="I4" s="2">
         <v>3.5162900000000002E-5</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="2"/>
+      <c r="K4" s="2">
         <v>6.2188300000000001E-6</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="11">
+      <c r="L4" s="2">
+        <v>7.2283589800322982E-6</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="11">
         <f>I4/H4</f>
         <v>0.99689086318468723</v>
       </c>
-      <c r="N4" s="11">
-        <f>J4/H4</f>
-        <v>0.17630783600609815</v>
-      </c>
-      <c r="O4" s="13">
-        <f>K4/H4</f>
+      <c r="Q4" s="11">
+        <f>L4/H4</f>
+        <v>0.20492863282076229</v>
+      </c>
+      <c r="R4" s="13">
+        <f>N4/H4</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>0.5</v>
       </c>
       <c r="B5" s="8">
-        <f>A5*$I$27</f>
+        <f>A5*$B$21</f>
         <v>0.20148367752532464</v>
       </c>
       <c r="C5" s="8">
@@ -611,30 +2365,35 @@
       <c r="I5" s="5">
         <v>1.7669699999999999E-4</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J5" s="5"/>
+      <c r="K5" s="5">
         <v>3.4790399999999998E-5</v>
       </c>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="9">
-        <f t="shared" ref="M5:M16" si="0">I5/H5</f>
+      <c r="L5" s="5">
+        <v>3.5506773449112674E-5</v>
+      </c>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="9">
+        <f t="shared" ref="P5:P16" si="0">I5/H5</f>
         <v>1.0034569826319439</v>
       </c>
-      <c r="N5" s="9">
-        <f t="shared" ref="N5:N16" si="1">J5/H5</f>
-        <v>0.19757364193256469</v>
-      </c>
-      <c r="O5" s="6">
-        <f t="shared" ref="O5:O16" si="2">K5/H5</f>
+      <c r="Q5" s="9">
+        <f t="shared" ref="Q5:Q16" si="1">L5/H5</f>
+        <v>0.20164190534215423</v>
+      </c>
+      <c r="R5" s="6">
+        <f t="shared" ref="R5:R16" si="2">N5/H5</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1.5</v>
       </c>
       <c r="B6" s="10">
-        <f>A6*$I$27</f>
+        <f>A6*$B$21</f>
         <v>0.60445103257597399</v>
       </c>
       <c r="C6" s="10">
@@ -653,30 +2412,35 @@
       <c r="I6" s="2">
         <v>5.2894699999999999E-4</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="2"/>
+      <c r="K6" s="2">
         <v>1.07774E-4</v>
       </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="11">
+      <c r="L6" s="2">
+        <v>1.0564601677004478E-4</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="11">
         <f t="shared" si="0"/>
         <v>1.0039855290430377</v>
       </c>
-      <c r="N6" s="11">
+      <c r="Q6" s="11">
         <f t="shared" si="1"/>
-        <v>0.20456404215750229</v>
-      </c>
-      <c r="O6" s="13">
+        <v>0.20052495247758861</v>
+      </c>
+      <c r="R6" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>15</v>
       </c>
       <c r="B7" s="8">
-        <f>A7*$I$27</f>
+        <f>A7*$B$21</f>
         <v>6.044510325759739</v>
       </c>
       <c r="C7" s="8">
@@ -695,30 +2459,35 @@
       <c r="I7" s="5">
         <v>5.0301599999999997E-3</v>
       </c>
-      <c r="J7" s="5">
+      <c r="J7" s="5"/>
+      <c r="K7" s="5">
         <v>9.837540000000001E-4</v>
       </c>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="9">
+      <c r="L7" s="5">
+        <v>1.0548236927556496E-3</v>
+      </c>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="9">
         <f t="shared" si="0"/>
         <v>1.0009554196724095</v>
       </c>
-      <c r="N7" s="9">
+      <c r="Q7" s="9">
         <f t="shared" si="1"/>
-        <v>0.1957579675247729</v>
-      </c>
-      <c r="O7" s="6">
+        <v>0.20990018052360801</v>
+      </c>
+      <c r="R7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>30</v>
       </c>
       <c r="B8" s="10">
-        <f>A8*$I$27</f>
+        <f>A8*$B$21</f>
         <v>12.089020651519478</v>
       </c>
       <c r="C8" s="10">
@@ -737,30 +2506,35 @@
       <c r="I8" s="2">
         <v>9.5466400000000003E-3</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="2"/>
+      <c r="K8" s="2">
         <v>1.9574700000000002E-3</v>
       </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="11">
+      <c r="L8" s="2">
+        <v>2.0948517588691182E-3</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="11">
         <f t="shared" si="0"/>
         <v>0.99344018879627238</v>
       </c>
-      <c r="N8" s="11">
+      <c r="Q8" s="11">
         <f t="shared" si="1"/>
-        <v>0.20369777915193613</v>
-      </c>
-      <c r="O8" s="13">
+        <v>0.21799396717914785</v>
+      </c>
+      <c r="R8" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>60</v>
       </c>
       <c r="B9" s="8">
-        <f>A9*$I$27</f>
+        <f>A9*$B$21</f>
         <v>24.178041303038956</v>
       </c>
       <c r="C9" s="8">
@@ -779,30 +2553,35 @@
       <c r="I9" s="5">
         <v>1.7839399999999998E-2</v>
       </c>
-      <c r="J9" s="5">
+      <c r="J9" s="5"/>
+      <c r="K9" s="5">
         <v>3.77656E-3</v>
       </c>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="9">
+      <c r="L9" s="5">
+        <v>4.108953764066098E-3</v>
+      </c>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="9">
         <f t="shared" si="0"/>
         <v>0.99349512228377224</v>
       </c>
-      <c r="N9" s="9">
+      <c r="Q9" s="9">
         <f t="shared" si="1"/>
-        <v>0.21032063516777488</v>
-      </c>
-      <c r="O9" s="6">
+        <v>0.22883199672013713</v>
+      </c>
+      <c r="R9" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>90</v>
       </c>
       <c r="B10" s="10">
-        <f>A10*$I$27</f>
+        <f>A10*$B$21</f>
         <v>36.267061954558436</v>
       </c>
       <c r="C10" s="10">
@@ -821,30 +2600,35 @@
       <c r="I10" s="2">
         <v>2.5426299999999999E-2</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="2"/>
+      <c r="K10" s="2">
         <v>5.35463E-3</v>
       </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="11">
+      <c r="L10" s="2">
+        <v>6.0812610365238457E-3</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="11">
         <f t="shared" si="0"/>
         <v>0.99821889366212679</v>
       </c>
-      <c r="N10" s="11">
+      <c r="Q10" s="11">
         <f t="shared" si="1"/>
-        <v>0.21021905800568838</v>
-      </c>
-      <c r="O10" s="13">
+        <v>0.23874608826095153</v>
+      </c>
+      <c r="R10" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>120</v>
       </c>
       <c r="B11" s="8">
-        <f>A11*$I$27</f>
+        <f>A11*$B$21</f>
         <v>48.356082606077912</v>
       </c>
       <c r="C11" s="8">
@@ -863,30 +2647,35 @@
       <c r="I11" s="5">
         <v>3.2291500000000001E-2</v>
       </c>
-      <c r="J11" s="5">
+      <c r="J11" s="5"/>
+      <c r="K11" s="5">
         <v>7.2558700000000002E-3</v>
       </c>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="9">
+      <c r="L11" s="5">
+        <v>8.017270967046913E-3</v>
+      </c>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="9">
         <f t="shared" si="0"/>
         <v>0.99610882134451439</v>
       </c>
-      <c r="N11" s="9">
+      <c r="Q11" s="9">
         <f t="shared" si="1"/>
-        <v>0.22382472519173843</v>
-      </c>
-      <c r="O11" s="6">
+        <v>0.24731196548270273</v>
+      </c>
+      <c r="R11" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>150</v>
       </c>
       <c r="B12" s="10">
-        <f>A12*$I$27</f>
+        <f>A12*$B$21</f>
         <v>60.445103257597395</v>
       </c>
       <c r="C12" s="10">
@@ -905,30 +2694,35 @@
       <c r="I12" s="2">
         <v>3.9017400000000001E-2</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="2"/>
+      <c r="K12" s="2">
         <v>8.6777399999999998E-3</v>
       </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="11">
+      <c r="L12" s="2">
+        <v>9.8697824484955642E-3</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="11">
         <f t="shared" si="0"/>
         <v>0.99903181082605086</v>
       </c>
-      <c r="N12" s="11">
+      <c r="Q12" s="11">
         <f t="shared" si="1"/>
-        <v>0.22219159416254425</v>
-      </c>
-      <c r="O12" s="13">
+        <v>0.25271357476355927</v>
+      </c>
+      <c r="R12" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>250</v>
       </c>
       <c r="B13" s="8">
-        <f>A13*$I$27</f>
+        <f>A13*$B$21</f>
         <v>100.74183876266233</v>
       </c>
       <c r="C13" s="8">
@@ -947,30 +2741,35 @@
       <c r="I13" s="5">
         <v>5.9058800000000002E-2</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5">
         <v>1.3802999999999999E-2</v>
       </c>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="9">
+      <c r="L13" s="5">
+        <v>1.5481580872935446E-2</v>
+      </c>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+      <c r="P13" s="9">
         <f t="shared" si="0"/>
         <v>1.001279618104651</v>
       </c>
-      <c r="N13" s="9">
+      <c r="Q13" s="9">
         <f t="shared" si="1"/>
-        <v>0.23401529608963434</v>
-      </c>
-      <c r="O13" s="6">
+        <v>0.26247386306713094</v>
+      </c>
+      <c r="R13" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>500</v>
       </c>
       <c r="B14" s="10">
-        <f>A14*$I$27</f>
+        <f>A14*$B$21</f>
         <v>201.48367752532465</v>
       </c>
       <c r="C14" s="10">
@@ -989,30 +2788,35 @@
       <c r="I14" s="2">
         <v>0.104042</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="2"/>
+      <c r="K14" s="2">
         <v>2.7241999999999999E-2</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="11">
+      <c r="L14" s="2">
+        <v>2.136209612868915E-2</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="11">
         <f t="shared" si="0"/>
         <v>1.0043140570534912</v>
       </c>
-      <c r="N14" s="11">
+      <c r="Q14" s="11">
         <f t="shared" si="1"/>
-        <v>0.2629661438866151</v>
-      </c>
-      <c r="O14" s="13">
+        <v>0.20620762221189981</v>
+      </c>
+      <c r="R14" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>750</v>
       </c>
       <c r="B15" s="8">
-        <f>A15*$I$27</f>
+        <f>A15*$B$21</f>
         <v>302.22551628798698</v>
       </c>
       <c r="C15" s="8">
@@ -1031,30 +2835,35 @@
       <c r="I15" s="5">
         <v>0.14546899999999999</v>
       </c>
-      <c r="J15" s="5">
+      <c r="J15" s="5"/>
+      <c r="K15" s="5">
         <v>3.7511500000000003E-2</v>
       </c>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="9">
+      <c r="L15" s="5">
+        <v>3.1478387405910621E-2</v>
+      </c>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="9">
         <f t="shared" si="0"/>
         <v>1.001891522935846</v>
       </c>
-      <c r="N15" s="9">
+      <c r="Q15" s="9">
         <f t="shared" si="1"/>
-        <v>0.25835369640684952</v>
-      </c>
-      <c r="O15" s="6">
+        <v>0.21680172062551026</v>
+      </c>
+      <c r="R15" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>1000</v>
       </c>
       <c r="B16" s="10">
-        <f>A16*$I$27</f>
+        <f>A16*$B$21</f>
         <v>402.9673550506493</v>
       </c>
       <c r="C16" s="10">
@@ -1074,62 +2883,90 @@
         <v>0.186667</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="M16" s="11">
+      <c r="K16" s="2"/>
+      <c r="L16" s="2">
+        <v>4.0537614166508758E-2</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="P16" s="11">
         <f t="shared" si="0"/>
         <v>1.0040173085979736</v>
       </c>
-      <c r="N16" s="11">
+      <c r="Q16" s="11">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="O16" s="13">
+        <v>0.21803782282053716</v>
+      </c>
+      <c r="R16" s="13">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H24" s="1" t="s">
-        <v>11</v>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="G25" s="1"/>
-      <c r="H25" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>6</v>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H26" t="s">
-        <v>8</v>
-      </c>
-      <c r="I26">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
         <f>4/3*PI()*(0.04)^3</f>
         <v>2.6808257310632905E-4</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H27" t="s">
-        <v>19</v>
-      </c>
-      <c r="I27">
-        <f>(238.02+32)/238.05 / I26 / 10.5 / 100^3 * 1000</f>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21">
+        <f>(238.02+32)/238.05 / B20 / 10.5 / 100^3 * 1000</f>
         <v>0.40296735505064929</v>
       </c>
     </row>
-    <row r="35" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="9:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="9:11" x14ac:dyDescent="0.3">
       <c r="I36" s="12"/>
+      <c r="J36" s="12"/>
+      <c r="K36" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD64C41-891F-45FF-892B-9697A9E85178}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>